<commit_message>
Sony Neural Network Console いろいろ試す編用
Sony Neural Network Console いろいろ試す編用
</commit_message>
<xml_diff>
--- a/NNC/weight_bias_alignment.xlsx
+++ b/NNC/weight_bias_alignment.xlsx
@@ -2,23 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\●ブログ用\neural\NNC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC739582-A308-4650-BC9C-7625054FDCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A1E58F-FDF3-4F2D-84A1-7C8ACBA048DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="5" xr2:uid="{A26ADE69-E7FC-4358-8ECF-736C24E7B46E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{A26ADE69-E7FC-4358-8ECF-736C24E7B46E}"/>
   </bookViews>
   <sheets>
-    <sheet name="convolution1" sheetId="10" r:id="rId1"/>
-    <sheet name="conv1_out" sheetId="11" r:id="rId2"/>
-    <sheet name="convolution2" sheetId="12" r:id="rId3"/>
-    <sheet name="conv2_out" sheetId="13" r:id="rId4"/>
-    <sheet name="affine" sheetId="8" r:id="rId5"/>
-    <sheet name="affine_out" sheetId="9" r:id="rId6"/>
+    <sheet name="conv1_貼り付け" sheetId="10" r:id="rId1"/>
+    <sheet name="conv1_整列" sheetId="11" r:id="rId2"/>
+    <sheet name="depthwise_conv_貼り付け" sheetId="12" r:id="rId3"/>
+    <sheet name="depthwise_conv_整列" sheetId="13" r:id="rId4"/>
+    <sheet name="affine_貼り付け" sheetId="8" r:id="rId5"/>
+    <sheet name="affine_整列" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -498,8 +493,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -525,144 +520,112 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.181940332055091</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>-0.27367174625396701</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>-1.0705676861107301E-2</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>-9.03233513236045E-2</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.22446142137050601</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
-        <v>-0.44727569818496699</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.29635366797447199</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="4">
         <v>4</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.28920495510101302</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.56113958358764604</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.72203731536865201</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="4">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.39657643437385498</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="4">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
-        <v>-1.19974145491141E-4</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>9.5103748142719199E-2</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>-0.11673650145530701</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>-1.05050420388579E-2</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="4">
         <v>4</v>
       </c>
-      <c r="C17" s="1">
-        <v>6.3451126217842102E-2</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -671,144 +634,112 @@
       <c r="B18" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
-        <v>-6.4163461327552795E-2</v>
-      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="1">
-        <v>-0.14576697349548301</v>
-      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="4">
         <v>3</v>
       </c>
-      <c r="C20" s="1">
-        <v>-0.163172751665115</v>
-      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="4">
         <v>4</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.29863455891609098</v>
-      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="1">
-        <v>8.4337368607521002E-2</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
-        <v>-7.3834940791129997E-2</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="4">
         <v>3</v>
       </c>
-      <c r="C24" s="1">
-        <v>-0.16018408536911</v>
-      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="4">
         <v>4</v>
       </c>
-      <c r="C25" s="1">
-        <v>-0.202994599938392</v>
-      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="4">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>0.175181403756141</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="4">
         <v>2</v>
       </c>
-      <c r="C27" s="1">
-        <v>-3.7168096750974599E-3</v>
-      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="1">
-        <v>8.9502066373825004E-2</v>
-      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="4">
         <v>4</v>
       </c>
-      <c r="C29" s="1">
-        <v>-0.155304715037345</v>
-      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="4">
         <v>1</v>
       </c>
-      <c r="C30" s="1">
-        <v>0.35284867882728499</v>
-      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="4">
         <v>2</v>
       </c>
-      <c r="C31" s="1">
-        <v>0.13130746781826</v>
-      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="C32" s="1">
-        <v>0.27910745143890298</v>
-      </c>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="4">
         <v>4</v>
       </c>
-      <c r="C33" s="1">
-        <v>0.20858530700206701</v>
-      </c>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
@@ -817,144 +748,112 @@
       <c r="B34" s="4">
         <v>1</v>
       </c>
-      <c r="C34" s="1">
-        <v>0.14807994663715299</v>
-      </c>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="4">
         <v>2</v>
       </c>
-      <c r="C35" s="1">
-        <v>0.43832632899284302</v>
-      </c>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="C36" s="1">
-        <v>0.621867775917053</v>
-      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="4">
         <v>4</v>
       </c>
-      <c r="C37" s="1">
-        <v>0.93994605541229204</v>
-      </c>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="4">
         <v>1</v>
       </c>
-      <c r="C38" s="1">
-        <v>-1.4721267223358101</v>
-      </c>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="4">
         <v>2</v>
       </c>
-      <c r="C39" s="1">
-        <v>-7.7161993831396103E-3</v>
-      </c>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="4">
         <v>3</v>
       </c>
-      <c r="C40" s="1">
-        <v>-1.2683602981269301E-2</v>
-      </c>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="4">
         <v>4</v>
       </c>
-      <c r="C41" s="1">
-        <v>-0.71697229146957397</v>
-      </c>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="4">
         <v>1</v>
       </c>
-      <c r="C42" s="1">
-        <v>3.1751923263072898E-2</v>
-      </c>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="4">
         <v>2</v>
       </c>
-      <c r="C43" s="1">
-        <v>-1.92207407951354</v>
-      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="4">
         <v>3</v>
       </c>
-      <c r="C44" s="1">
-        <v>-1.2362186908721899</v>
-      </c>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="4">
         <v>4</v>
       </c>
-      <c r="C45" s="1">
-        <v>-0.136057138442993</v>
-      </c>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="4">
         <v>1</v>
       </c>
-      <c r="C46" s="1">
-        <v>-0.34056931734085</v>
-      </c>
+      <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="4">
         <v>2</v>
       </c>
-      <c r="C47" s="1">
-        <v>0.758761227130889</v>
-      </c>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="4">
         <v>3</v>
       </c>
-      <c r="C48" s="1">
-        <v>0.22130963206291199</v>
-      </c>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="4">
         <v>4</v>
       </c>
-      <c r="C49" s="1">
-        <v>0.21096575260162301</v>
-      </c>
+      <c r="C49" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -974,7 +873,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -983,196 +882,94 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.181940332055091</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-0.27367174625396701</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-1.0705676861107301E-2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>-9.03233513236045E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-2.23595690727233</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="1">
-        <v>0.22446142137050601</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-0.44727569818496699</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.29635366797447199</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.28920495510101302</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="1">
-        <v>0.56113958358764604</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.72203731536865201</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.39657643437385498</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-1.19974145491141E-4</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="1">
-        <v>9.5103748142719199E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-0.11673650145530701</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-1.05050420388579E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>6.3451126217842102E-2</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>-6.4163461327552795E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-0.14576697349548301</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-0.163172751665115</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-0.29863455891609098</v>
-      </c>
-      <c r="F6" s="1">
-        <v>-0.108140669763088</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="1">
-        <v>8.4337368607521002E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>-7.3834940791129997E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-0.16018408536911</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-0.202994599938392</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="1">
-        <v>0.175181403756141</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-3.7168096750974599E-3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8.9502066373825004E-2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-0.155304715037345</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="1">
-        <v>0.35284867882728499</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.13130746781826</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.27910745143890298</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.20858530700206701</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.14807994663715299</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.43832632899284302</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.621867775917053</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.93994605541229204</v>
-      </c>
-      <c r="F10" s="1">
-        <v>-1.0091449022293</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
-      <c r="B11" s="1">
-        <v>-1.4721267223358101</v>
-      </c>
-      <c r="C11" s="1">
-        <v>-7.7161993831396103E-3</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-1.2683602981269301E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-0.71697229146957397</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="1">
-        <v>3.1751923263072898E-2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1.92207407951354</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-1.2362186908721899</v>
-      </c>
-      <c r="E12" s="1">
-        <v>-0.136057138442993</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="1">
-        <v>-0.34056931734085</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.758761227130889</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.22130963206291199</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.21096575260162301</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1182,6 +979,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1191,7 +989,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1217,81 +1015,63 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.27820703387260398</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>-0.278210818767547</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>-1.2405359745025599</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>5.4196026176214197E-2</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>-0.53386956453323298</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
-        <v>-0.23294465243816301</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>2.16198205947875</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.72202056646347001</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.48038727045059199</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
@@ -1300,81 +1080,63 @@
       <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.53832882642745905</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.74220603704452504</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="4">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
-        <v>1.65692722797393</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.363009303808212</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>-5.3189747035503297E-2</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>-0.36557790637016202</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C17" s="1">
-        <v>0.112545445561409</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="1">
-        <v>6.4462982118129702E-2</v>
-      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="4">
         <v>3</v>
       </c>
-      <c r="C19" s="1">
-        <v>-0.72223210334777799</v>
-      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1383,81 +1145,63 @@
       <c r="B20" s="4">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.230633214116096</v>
-      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="1">
-        <v>0.22468791902065199</v>
-      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="4">
         <v>3</v>
       </c>
-      <c r="C22" s="1">
-        <v>-0.100684858858585</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="4">
         <v>1</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.55528730154037398</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="1">
-        <v>0.48822098970413202</v>
-      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="4">
         <v>3</v>
       </c>
-      <c r="C25" s="1">
-        <v>-0.107516810297966</v>
-      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="4">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>0.230024963617324</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="4">
         <v>2</v>
       </c>
-      <c r="C27" s="1">
-        <v>-0.25984388589858998</v>
-      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="1">
-        <v>-0.23848533630370999</v>
-      </c>
+      <c r="C28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1467,6 +1211,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1476,7 +1221,7 @@
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1485,124 +1230,64 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.27820703387260398</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-0.278210818767547</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-1.2405359745025599</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.56218951940536499</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="1">
-        <v>5.4196026176214197E-2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-0.53386956453323298</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-0.23294465243816301</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="1">
-        <v>2.16198205947875</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.72202056646347001</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.48038727045059199</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.53832882642745905</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.74220603704452504</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.65692722797393</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-1.64633905887603</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="1">
-        <v>0.363009303808212</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-5.3189747035503297E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-0.36557790637016202</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="1">
-        <v>0.112545445561409</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.4462982118129702E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-0.72223210334777799</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.230633214116096</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.22468791902065199</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-0.100684858858585</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.18459901213645899</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="1">
-        <v>0.55528730154037398</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.48822098970413202</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-0.107516810297966</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="1">
-        <v>0.230024963617324</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-0.25984388589858998</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-0.23848533630370999</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1612,6 +1297,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1621,7 +1307,7 @@
   <dimension ref="A1:O121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D121"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1654,9 +1340,7 @@
       <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>-0.40052118897437999</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1664,9 +1348,7 @@
       <c r="C3" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
-        <v>-0.50818932056427002</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
@@ -1674,9 +1356,7 @@
       <c r="C4" s="6">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
-        <v>1.6067522764205899</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
@@ -1684,9 +1364,7 @@
       <c r="C5" s="6">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
-        <v>1.42947030067443</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
@@ -1696,9 +1374,7 @@
       <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
-        <v>4.9180030822753897</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1706,9 +1382,7 @@
       <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
-        <v>-0.90105837583541804</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
@@ -1716,9 +1390,7 @@
       <c r="C8" s="6">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
-        <v>2.78665900230407</v>
-      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -1726,9 +1398,7 @@
       <c r="C9" s="6">
         <v>4</v>
       </c>
-      <c r="D9" s="1">
-        <v>-1.8359341621398899</v>
-      </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
@@ -1738,9 +1408,7 @@
       <c r="C10" s="6">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <v>-5.10003232955932</v>
-      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1748,9 +1416,7 @@
       <c r="C11" s="6">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
-        <v>0.82219988107681197</v>
-      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1758,9 +1424,7 @@
       <c r="C12" s="6">
         <v>3</v>
       </c>
-      <c r="D12" s="1">
-        <v>-6.7797913551330504</v>
-      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1768,9 +1432,7 @@
       <c r="C13" s="6">
         <v>4</v>
       </c>
-      <c r="D13" s="1">
-        <v>6.9477461278438499E-2</v>
-      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -1782,9 +1444,7 @@
       <c r="C14" s="6">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
-        <v>-1.0582468509673999</v>
-      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1792,9 +1452,7 @@
       <c r="C15" s="6">
         <v>2</v>
       </c>
-      <c r="D15" s="1">
-        <v>-3.8543810844421298</v>
-      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -1802,9 +1460,7 @@
       <c r="C16" s="6">
         <v>3</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.67772495746612504</v>
-      </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
@@ -1812,9 +1468,7 @@
       <c r="C17" s="6">
         <v>4</v>
       </c>
-      <c r="D17" s="1">
-        <v>-2.1101441383361799</v>
-      </c>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -1824,9 +1478,7 @@
       <c r="C18" s="6">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
-        <v>-2.8954362869262602</v>
-      </c>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1834,9 +1486,7 @@
       <c r="C19" s="6">
         <v>2</v>
       </c>
-      <c r="D19" s="1">
-        <v>-3.0784225463867099</v>
-      </c>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
@@ -1844,9 +1494,7 @@
       <c r="C20" s="6">
         <v>3</v>
       </c>
-      <c r="D20" s="1">
-        <v>3.0786654949188201</v>
-      </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
@@ -1854,9 +1502,7 @@
       <c r="C21" s="6">
         <v>4</v>
       </c>
-      <c r="D21" s="1">
-        <v>-1.2044198513030999</v>
-      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
@@ -1866,9 +1512,7 @@
       <c r="C22" s="6">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>2.5151956081390301</v>
-      </c>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
@@ -1876,9 +1520,7 @@
       <c r="C23" s="6">
         <v>2</v>
       </c>
-      <c r="D23" s="1">
-        <v>-4.8810110092162997</v>
-      </c>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
@@ -1886,9 +1528,7 @@
       <c r="C24" s="6">
         <v>3</v>
       </c>
-      <c r="D24" s="1">
-        <v>-0.96713423728942804</v>
-      </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
@@ -1896,9 +1536,7 @@
       <c r="C25" s="6">
         <v>4</v>
       </c>
-      <c r="D25" s="1">
-        <v>-2.9760582447052002</v>
-      </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -1910,9 +1548,7 @@
       <c r="C26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="1">
-        <v>0.94170200824737504</v>
-      </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
@@ -1920,9 +1556,7 @@
       <c r="C27" s="6">
         <v>2</v>
       </c>
-      <c r="D27" s="1">
-        <v>-1.1237534284591599</v>
-      </c>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
@@ -1930,9 +1564,7 @@
       <c r="C28" s="6">
         <v>3</v>
       </c>
-      <c r="D28" s="1">
-        <v>0.109016112983226</v>
-      </c>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
@@ -1940,9 +1572,7 @@
       <c r="C29" s="6">
         <v>4</v>
       </c>
-      <c r="D29" s="1">
-        <v>0.27482166886329601</v>
-      </c>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
@@ -1952,9 +1582,7 @@
       <c r="C30" s="6">
         <v>1</v>
       </c>
-      <c r="D30" s="1">
-        <v>1.45249712467193</v>
-      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
@@ -1962,9 +1590,7 @@
       <c r="C31" s="6">
         <v>2</v>
       </c>
-      <c r="D31" s="1">
-        <v>-0.953480005264282</v>
-      </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
@@ -1972,9 +1598,7 @@
       <c r="C32" s="6">
         <v>3</v>
       </c>
-      <c r="D32" s="1">
-        <v>2.0774867534637398</v>
-      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
@@ -1982,9 +1606,7 @@
       <c r="C33" s="6">
         <v>4</v>
       </c>
-      <c r="D33" s="1">
-        <v>2.0978410243988002</v>
-      </c>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
@@ -1994,9 +1616,7 @@
       <c r="C34" s="6">
         <v>1</v>
       </c>
-      <c r="D34" s="1">
-        <v>4.6142249107360804</v>
-      </c>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
@@ -2004,9 +1624,7 @@
       <c r="C35" s="6">
         <v>2</v>
       </c>
-      <c r="D35" s="5">
-        <v>0.24730111658573101</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -2015,9 +1633,7 @@
       <c r="C36" s="6">
         <v>3</v>
       </c>
-      <c r="D36" s="1">
-        <v>-3.11406350135803</v>
-      </c>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
@@ -2025,9 +1641,7 @@
       <c r="C37" s="6">
         <v>4</v>
       </c>
-      <c r="D37" s="1">
-        <v>-0.51415812969207697</v>
-      </c>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
@@ -2039,9 +1653,7 @@
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="1">
-        <v>-1.1968530416488601</v>
-      </c>
+      <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
@@ -2049,9 +1661,7 @@
       <c r="C39" s="6">
         <v>2</v>
       </c>
-      <c r="D39" s="1">
-        <v>0.158195599913597</v>
-      </c>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
@@ -2059,9 +1669,7 @@
       <c r="C40" s="6">
         <v>3</v>
       </c>
-      <c r="D40" s="1">
-        <v>2.0046212673187198</v>
-      </c>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
@@ -2069,9 +1677,7 @@
       <c r="C41" s="6">
         <v>4</v>
       </c>
-      <c r="D41" s="1">
-        <v>1.7418861389160101</v>
-      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
@@ -2081,9 +1687,7 @@
       <c r="C42" s="6">
         <v>1</v>
       </c>
-      <c r="D42" s="1">
-        <v>-3.4003209322690901E-2</v>
-      </c>
+      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
@@ -2091,9 +1695,7 @@
       <c r="C43" s="6">
         <v>2</v>
       </c>
-      <c r="D43" s="1">
-        <v>-0.35034716129302901</v>
-      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
@@ -2101,9 +1703,7 @@
       <c r="C44" s="6">
         <v>3</v>
       </c>
-      <c r="D44" s="1">
-        <v>-0.90647095441818204</v>
-      </c>
+      <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
@@ -2111,9 +1711,7 @@
       <c r="C45" s="6">
         <v>4</v>
       </c>
-      <c r="D45" s="1">
-        <v>-1.1158876419067301</v>
-      </c>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
@@ -2123,9 +1721,7 @@
       <c r="C46" s="6">
         <v>1</v>
       </c>
-      <c r="D46" s="1">
-        <v>5.34647464752197</v>
-      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
@@ -2133,9 +1729,7 @@
       <c r="C47" s="6">
         <v>2</v>
       </c>
-      <c r="D47" s="1">
-        <v>-0.64035367965698198</v>
-      </c>
+      <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
@@ -2143,9 +1737,7 @@
       <c r="C48" s="6">
         <v>3</v>
       </c>
-      <c r="D48" s="1">
-        <v>1.7845815420150699</v>
-      </c>
+      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
@@ -2153,9 +1745,7 @@
       <c r="C49" s="6">
         <v>4</v>
       </c>
-      <c r="D49" s="1">
-        <v>2.5202553272247301</v>
-      </c>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
@@ -2167,9 +1757,7 @@
       <c r="C50" s="6">
         <v>1</v>
       </c>
-      <c r="D50" s="1">
-        <v>2.6735858917236301</v>
-      </c>
+      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
@@ -2177,9 +1765,7 @@
       <c r="C51" s="6">
         <v>2</v>
       </c>
-      <c r="D51" s="1">
-        <v>2.71317434310913</v>
-      </c>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
@@ -2187,9 +1773,7 @@
       <c r="C52" s="6">
         <v>3</v>
       </c>
-      <c r="D52" s="1">
-        <v>-2.1070787906646702</v>
-      </c>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
@@ -2197,9 +1781,7 @@
       <c r="C53" s="6">
         <v>4</v>
       </c>
-      <c r="D53" s="1">
-        <v>-2.7435026168823198</v>
-      </c>
+      <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
@@ -2209,9 +1791,7 @@
       <c r="C54" s="6">
         <v>1</v>
       </c>
-      <c r="D54" s="1">
-        <v>-1.7146010398864699</v>
-      </c>
+      <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
@@ -2219,9 +1799,7 @@
       <c r="C55" s="6">
         <v>2</v>
       </c>
-      <c r="D55" s="1">
-        <v>-1.3054788112640301</v>
-      </c>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
@@ -2229,9 +1807,7 @@
       <c r="C56" s="6">
         <v>3</v>
       </c>
-      <c r="D56" s="1">
-        <v>1.95961225032806</v>
-      </c>
+      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
@@ -2239,9 +1815,7 @@
       <c r="C57" s="6">
         <v>4</v>
       </c>
-      <c r="D57" s="1">
-        <v>-1.1790909767150799</v>
-      </c>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
@@ -2251,9 +1825,7 @@
       <c r="C58" s="6">
         <v>1</v>
       </c>
-      <c r="D58" s="1">
-        <v>-4.2376422882079998</v>
-      </c>
+      <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
@@ -2261,9 +1833,7 @@
       <c r="C59" s="6">
         <v>2</v>
       </c>
-      <c r="D59" s="1">
-        <v>-4.1689424514770499</v>
-      </c>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
@@ -2271,9 +1841,7 @@
       <c r="C60" s="6">
         <v>3</v>
       </c>
-      <c r="D60" s="1">
-        <v>1.36287653446197</v>
-      </c>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
@@ -2281,9 +1849,7 @@
       <c r="C61" s="6">
         <v>4</v>
       </c>
-      <c r="D61" s="1">
-        <v>-1.6322774887084901</v>
-      </c>
+      <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
@@ -2295,9 +1861,7 @@
       <c r="C62" s="6">
         <v>1</v>
       </c>
-      <c r="D62" s="1">
-        <v>-0.55348229408264105</v>
-      </c>
+      <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
@@ -2305,9 +1869,7 @@
       <c r="C63" s="6">
         <v>2</v>
       </c>
-      <c r="D63" s="1">
-        <v>-2.2128365039825399</v>
-      </c>
+      <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
@@ -2315,9 +1877,7 @@
       <c r="C64" s="6">
         <v>3</v>
       </c>
-      <c r="D64" s="1">
-        <v>0.28832209110259999</v>
-      </c>
+      <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
@@ -2325,9 +1885,7 @@
       <c r="C65" s="6">
         <v>4</v>
       </c>
-      <c r="D65" s="1">
-        <v>2.4534537792205802</v>
-      </c>
+      <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
@@ -2337,9 +1895,7 @@
       <c r="C66" s="6">
         <v>1</v>
       </c>
-      <c r="D66" s="1">
-        <v>-2.8020896911621</v>
-      </c>
+      <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
@@ -2347,9 +1903,7 @@
       <c r="C67" s="6">
         <v>2</v>
       </c>
-      <c r="D67" s="1">
-        <v>3.5175354480743399</v>
-      </c>
+      <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
@@ -2357,9 +1911,7 @@
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="D68" s="1">
-        <v>-0.927859187126159</v>
-      </c>
+      <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
@@ -2367,9 +1919,7 @@
       <c r="C69" s="6">
         <v>4</v>
       </c>
-      <c r="D69" s="1">
-        <v>2.147394657135</v>
-      </c>
+      <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
@@ -2379,9 +1929,7 @@
       <c r="C70" s="6">
         <v>1</v>
       </c>
-      <c r="D70" s="1">
-        <v>-2.05948615074157</v>
-      </c>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
@@ -2389,9 +1937,7 @@
       <c r="C71" s="6">
         <v>2</v>
       </c>
-      <c r="D71" s="1">
-        <v>2.5537962913513099</v>
-      </c>
+      <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
@@ -2399,9 +1945,7 @@
       <c r="C72" s="6">
         <v>3</v>
       </c>
-      <c r="D72" s="1">
-        <v>1.53719794750213</v>
-      </c>
+      <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
@@ -2409,9 +1953,7 @@
       <c r="C73" s="6">
         <v>4</v>
       </c>
-      <c r="D73" s="1">
-        <v>2.43905448913574</v>
-      </c>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -2423,9 +1965,7 @@
       <c r="C74" s="6">
         <v>1</v>
       </c>
-      <c r="D74" s="1">
-        <v>2.04607701301574</v>
-      </c>
+      <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
@@ -2433,9 +1973,7 @@
       <c r="C75" s="6">
         <v>2</v>
       </c>
-      <c r="D75" s="1">
-        <v>0.66513007879257202</v>
-      </c>
+      <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
@@ -2443,9 +1981,7 @@
       <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="D76" s="1">
-        <v>-2.6995031833648602</v>
-      </c>
+      <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
@@ -2453,9 +1989,7 @@
       <c r="C77" s="6">
         <v>4</v>
       </c>
-      <c r="D77" s="1">
-        <v>2.3459839820861799</v>
-      </c>
+      <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
@@ -2465,9 +1999,7 @@
       <c r="C78" s="6">
         <v>1</v>
       </c>
-      <c r="D78" s="1">
-        <v>-7.10182428359985</v>
-      </c>
+      <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
@@ -2475,9 +2007,7 @@
       <c r="C79" s="6">
         <v>2</v>
       </c>
-      <c r="D79" s="1">
-        <v>3.30178475379943</v>
-      </c>
+      <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
@@ -2485,9 +2015,7 @@
       <c r="C80" s="6">
         <v>3</v>
       </c>
-      <c r="D80" s="1">
-        <v>1.6101393699645901</v>
-      </c>
+      <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
@@ -2495,9 +2023,7 @@
       <c r="C81" s="6">
         <v>4</v>
       </c>
-      <c r="D81" s="1">
-        <v>4.0910239219665501</v>
-      </c>
+      <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
@@ -2507,9 +2033,7 @@
       <c r="C82" s="6">
         <v>1</v>
       </c>
-      <c r="D82" s="1">
-        <v>-9.42006111145019</v>
-      </c>
+      <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
@@ -2517,9 +2041,7 @@
       <c r="C83" s="6">
         <v>2</v>
       </c>
-      <c r="D83" s="1">
-        <v>-0.65038734674453702</v>
-      </c>
+      <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
@@ -2527,9 +2049,7 @@
       <c r="C84" s="6">
         <v>3</v>
       </c>
-      <c r="D84" s="1">
-        <v>-6.3610930442809996</v>
-      </c>
+      <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
@@ -2537,9 +2057,7 @@
       <c r="C85" s="6">
         <v>4</v>
       </c>
-      <c r="D85" s="1">
-        <v>1.8409708738327</v>
-      </c>
+      <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
@@ -2551,9 +2069,7 @@
       <c r="C86" s="6">
         <v>1</v>
       </c>
-      <c r="D86" s="1">
-        <v>-1.0775576829910201</v>
-      </c>
+      <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
@@ -2561,9 +2077,7 @@
       <c r="C87" s="6">
         <v>2</v>
       </c>
-      <c r="D87" s="1">
-        <v>-2.7043211460113499</v>
-      </c>
+      <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
@@ -2571,9 +2085,7 @@
       <c r="C88" s="6">
         <v>3</v>
       </c>
-      <c r="D88" s="1">
-        <v>0.133634358644485</v>
-      </c>
+      <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
@@ -2581,9 +2093,7 @@
       <c r="C89" s="6">
         <v>4</v>
       </c>
-      <c r="D89" s="1">
-        <v>-4.8889384269714302</v>
-      </c>
+      <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
@@ -2593,9 +2103,7 @@
       <c r="C90" s="6">
         <v>1</v>
       </c>
-      <c r="D90" s="1">
-        <v>6.9969301223754803</v>
-      </c>
+      <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
@@ -2603,9 +2111,7 @@
       <c r="C91" s="6">
         <v>2</v>
       </c>
-      <c r="D91" s="1">
-        <v>-1.65060234069824</v>
-      </c>
+      <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
@@ -2613,9 +2119,7 @@
       <c r="C92" s="6">
         <v>3</v>
       </c>
-      <c r="D92" s="1">
-        <v>-3.4171557426452601</v>
-      </c>
+      <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
@@ -2623,9 +2127,7 @@
       <c r="C93" s="6">
         <v>4</v>
       </c>
-      <c r="D93" s="1">
-        <v>1.83386671543121</v>
-      </c>
+      <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
@@ -2635,9 +2137,7 @@
       <c r="C94" s="6">
         <v>1</v>
       </c>
-      <c r="D94" s="1">
-        <v>3.2007508277893</v>
-      </c>
+      <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="7"/>
@@ -2645,9 +2145,7 @@
       <c r="C95" s="6">
         <v>2</v>
       </c>
-      <c r="D95" s="1">
-        <v>1.91202569007873</v>
-      </c>
+      <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="7"/>
@@ -2655,9 +2153,7 @@
       <c r="C96" s="6">
         <v>3</v>
       </c>
-      <c r="D96" s="1">
-        <v>1.7085886001586901</v>
-      </c>
+      <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="7"/>
@@ -2665,9 +2161,7 @@
       <c r="C97" s="6">
         <v>4</v>
       </c>
-      <c r="D97" s="1">
-        <v>-2.5924918651580802</v>
-      </c>
+      <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -2679,9 +2173,7 @@
       <c r="C98" s="6">
         <v>1</v>
       </c>
-      <c r="D98" s="1">
-        <v>-0.59897530078887895</v>
-      </c>
+      <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
@@ -2689,9 +2181,7 @@
       <c r="C99" s="6">
         <v>2</v>
       </c>
-      <c r="D99" s="1">
-        <v>2.3569996356964098</v>
-      </c>
+      <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
@@ -2699,9 +2189,7 @@
       <c r="C100" s="6">
         <v>3</v>
       </c>
-      <c r="D100" s="1">
-        <v>-1.3289710283279399</v>
-      </c>
+      <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
@@ -2709,9 +2197,7 @@
       <c r="C101" s="6">
         <v>4</v>
       </c>
-      <c r="D101" s="1">
-        <v>2.7057578563690101</v>
-      </c>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
@@ -2721,9 +2207,7 @@
       <c r="C102" s="6">
         <v>1</v>
       </c>
-      <c r="D102" s="1">
-        <v>-0.67250257730483998</v>
-      </c>
+      <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
@@ -2731,9 +2215,7 @@
       <c r="C103" s="6">
         <v>2</v>
       </c>
-      <c r="D103" s="1">
-        <v>3.5115864276885902</v>
-      </c>
+      <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
@@ -2741,9 +2223,7 @@
       <c r="C104" s="6">
         <v>3</v>
       </c>
-      <c r="D104" s="1">
-        <v>-3.0443739891052202</v>
-      </c>
+      <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
@@ -2751,9 +2231,7 @@
       <c r="C105" s="6">
         <v>4</v>
       </c>
-      <c r="D105" s="1">
-        <v>-0.34232163429260198</v>
-      </c>
+      <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
@@ -2763,9 +2241,7 @@
       <c r="C106" s="6">
         <v>1</v>
       </c>
-      <c r="D106" s="1">
-        <v>1.5171325206756501</v>
-      </c>
+      <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
@@ -2773,9 +2249,7 @@
       <c r="C107" s="6">
         <v>2</v>
       </c>
-      <c r="D107" s="1">
-        <v>0.43526506423950101</v>
-      </c>
+      <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
@@ -2783,9 +2257,7 @@
       <c r="C108" s="6">
         <v>3</v>
       </c>
-      <c r="D108" s="1">
-        <v>-2.2962193489074698</v>
-      </c>
+      <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
@@ -2793,9 +2265,7 @@
       <c r="C109" s="6">
         <v>4</v>
       </c>
-      <c r="D109" s="1">
-        <v>-0.17438523471355399</v>
-      </c>
+      <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -2807,9 +2277,7 @@
       <c r="C110" s="6">
         <v>1</v>
       </c>
-      <c r="D110" s="1">
-        <v>-1.70358073711395</v>
-      </c>
+      <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
@@ -2817,9 +2285,7 @@
       <c r="C111" s="6">
         <v>2</v>
       </c>
-      <c r="D111" s="1">
-        <v>2.4219911098480198</v>
-      </c>
+      <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
@@ -2827,9 +2293,7 @@
       <c r="C112" s="6">
         <v>3</v>
       </c>
-      <c r="D112" s="1">
-        <v>-9.9958568811416598E-2</v>
-      </c>
+      <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
@@ -2837,9 +2301,7 @@
       <c r="C113" s="6">
         <v>4</v>
       </c>
-      <c r="D113" s="1">
-        <v>-2.54979276657104</v>
-      </c>
+      <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
@@ -2849,9 +2311,7 @@
       <c r="C114" s="6">
         <v>1</v>
       </c>
-      <c r="D114" s="1">
-        <v>3.8382477760314901</v>
-      </c>
+      <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
@@ -2859,9 +2319,7 @@
       <c r="C115" s="6">
         <v>2</v>
       </c>
-      <c r="D115" s="1">
-        <v>-2.5205166339874201</v>
-      </c>
+      <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
@@ -2869,9 +2327,7 @@
       <c r="C116" s="6">
         <v>3</v>
       </c>
-      <c r="D116" s="1">
-        <v>-0.67971986532211304</v>
-      </c>
+      <c r="D116" s="1"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
@@ -2879,9 +2335,7 @@
       <c r="C117" s="6">
         <v>4</v>
       </c>
-      <c r="D117" s="1">
-        <v>-3.2891609668731601</v>
-      </c>
+      <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
@@ -2891,9 +2345,7 @@
       <c r="C118" s="6">
         <v>1</v>
       </c>
-      <c r="D118" s="1">
-        <v>-1.7507747411727901</v>
-      </c>
+      <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
@@ -2901,9 +2353,7 @@
       <c r="C119" s="6">
         <v>2</v>
       </c>
-      <c r="D119" s="1">
-        <v>2.2773973941802899</v>
-      </c>
+      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
@@ -2911,9 +2361,7 @@
       <c r="C120" s="6">
         <v>3</v>
       </c>
-      <c r="D120" s="1">
-        <v>4.4582104682922301</v>
-      </c>
+      <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
@@ -2921,9 +2369,7 @@
       <c r="C121" s="6">
         <v>4</v>
       </c>
-      <c r="D121" s="1">
-        <v>-1.760959982872</v>
-      </c>
+      <c r="D121" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -2970,6 +2416,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2978,8 +2425,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2991,69 +2438,43 @@
       <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>-0.40052118897437999</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-0.50818932056427002</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.2597515583038299</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="1">
-        <v>1.6067522764205899</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.42947030067443</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>4.9180030822753897</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-0.90105837583541804</v>
-      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="1">
-        <v>2.78665900230407</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-1.8359341621398899</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
-        <v>-5.10003232955932</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.82219988107681197</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="1">
-        <v>-6.7797913551330504</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.9477461278438499E-2</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -3062,69 +2483,43 @@
       <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>-1.0582468509673999</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-3.8543810844421298</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-0.57230079174041704</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="1">
-        <v>0.67772495746612504</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-2.1101441383361799</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
-        <v>-2.8954362869262602</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-3.0784225463867099</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="1">
-        <v>3.0786654949188201</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-1.2044198513030999</v>
-      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="8">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
-        <v>2.5151956081390301</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-4.8810110092162997</v>
-      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="1">
-        <v>-0.96713423728942804</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-2.9760582447052002</v>
-      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -3133,69 +2528,43 @@
       <c r="B14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.94170200824737504</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-1.1237534284591599</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5.3418302536010698</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="1">
-        <v>0.109016112983226</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.27482166886329601</v>
-      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="8">
         <v>2</v>
       </c>
-      <c r="C16" s="1">
-        <v>1.45249712467193</v>
-      </c>
-      <c r="D16" s="1">
-        <v>-0.953480005264282</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="1">
-        <v>2.0774867534637398</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2.0978410243988002</v>
-      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="8">
         <v>3</v>
       </c>
-      <c r="C18" s="1">
-        <v>4.6142249107360804</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.24730111658573101</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="1">
-        <v>-3.11406350135803</v>
-      </c>
-      <c r="D19" s="1">
-        <v>-0.51415812969207697</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -3204,69 +2573,43 @@
       <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
-        <v>-1.1968530416488601</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.158195599913597</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.33246177434921198</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="1">
-        <v>2.0046212673187198</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1.7418861389160101</v>
-      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>2</v>
       </c>
-      <c r="C22" s="1">
-        <v>-3.4003209322690901E-2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>-0.35034716129302901</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="1">
-        <v>-0.90647095441818204</v>
-      </c>
-      <c r="D23" s="1">
-        <v>-1.1158876419067301</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="8">
         <v>3</v>
       </c>
-      <c r="C24" s="1">
-        <v>5.34647464752197</v>
-      </c>
-      <c r="D24" s="1">
-        <v>-0.64035367965698198</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="1">
-        <v>1.7845815420150699</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2.5202553272247301</v>
-      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -3275,69 +2618,43 @@
       <c r="B26" s="8">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>2.6735858917236301</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2.71317434310913</v>
-      </c>
-      <c r="E26" s="1">
-        <v>-4.9291124343871999</v>
-      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="1">
-        <v>-2.1070787906646702</v>
-      </c>
-      <c r="D27" s="1">
-        <v>-2.7435026168823198</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="8">
         <v>2</v>
       </c>
-      <c r="C28" s="1">
-        <v>-1.7146010398864699</v>
-      </c>
-      <c r="D28" s="1">
-        <v>-1.3054788112640301</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="1">
-        <v>1.95961225032806</v>
-      </c>
-      <c r="D29" s="1">
-        <v>-1.1790909767150799</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="8">
         <v>3</v>
       </c>
-      <c r="C30" s="1">
-        <v>-4.2376422882079998</v>
-      </c>
-      <c r="D30" s="1">
-        <v>-4.1689424514770499</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="1">
-        <v>1.36287653446197</v>
-      </c>
-      <c r="D31" s="1">
-        <v>-1.6322774887084901</v>
-      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
@@ -3346,69 +2663,43 @@
       <c r="B32" s="8">
         <v>1</v>
       </c>
-      <c r="C32" s="1">
-        <v>-0.55348229408264105</v>
-      </c>
-      <c r="D32" s="1">
-        <v>-2.2128365039825399</v>
-      </c>
-      <c r="E32" s="1">
-        <v>3.3111200332641602</v>
-      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="1">
-        <v>0.28832209110259999</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2.4534537792205802</v>
-      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>2</v>
       </c>
-      <c r="C34" s="1">
-        <v>-2.8020896911621</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3.5175354480743399</v>
-      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="1">
-        <v>-0.927859187126159</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2.147394657135</v>
-      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>3</v>
       </c>
-      <c r="C36" s="1">
-        <v>-2.05948615074157</v>
-      </c>
-      <c r="D36" s="1">
-        <v>2.5537962913513099</v>
-      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="1">
-        <v>1.53719794750213</v>
-      </c>
-      <c r="D37" s="1">
-        <v>2.43905448913574</v>
-      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
@@ -3417,69 +2708,43 @@
       <c r="B38" s="8">
         <v>1</v>
       </c>
-      <c r="C38" s="1">
-        <v>2.04607701301574</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0.66513007879257202</v>
-      </c>
-      <c r="E38" s="1">
-        <v>-1.9778907299041699</v>
-      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="9"/>
-      <c r="C39" s="1">
-        <v>-2.6995031833648602</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2.3459839820861799</v>
-      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
-      <c r="C40" s="1">
-        <v>-7.10182428359985</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3.30178475379943</v>
-      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="9"/>
-      <c r="C41" s="1">
-        <v>1.6101393699645901</v>
-      </c>
-      <c r="D41" s="1">
-        <v>4.0910239219665501</v>
-      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="8">
         <v>3</v>
       </c>
-      <c r="C42" s="1">
-        <v>-9.42006111145019</v>
-      </c>
-      <c r="D42" s="1">
-        <v>-0.65038734674453702</v>
-      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="9"/>
-      <c r="C43" s="1">
-        <v>-6.3610930442809996</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1.8409708738327</v>
-      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -3488,69 +2753,43 @@
       <c r="B44" s="8">
         <v>1</v>
       </c>
-      <c r="C44" s="1">
-        <v>-1.0775576829910201</v>
-      </c>
-      <c r="D44" s="1">
-        <v>-2.7043211460113499</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0.76492959260940496</v>
-      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="9"/>
-      <c r="C45" s="1">
-        <v>0.133634358644485</v>
-      </c>
-      <c r="D45" s="1">
-        <v>-4.8889384269714302</v>
-      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="8">
         <v>2</v>
       </c>
-      <c r="C46" s="1">
-        <v>6.9969301223754803</v>
-      </c>
-      <c r="D46" s="1">
-        <v>-1.65060234069824</v>
-      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="1">
-        <v>-3.4171557426452601</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1.83386671543121</v>
-      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="8">
         <v>3</v>
       </c>
-      <c r="C48" s="1">
-        <v>3.2007508277893</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1.91202569007873</v>
-      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="9"/>
-      <c r="C49" s="1">
-        <v>1.7085886001586901</v>
-      </c>
-      <c r="D49" s="1">
-        <v>-2.5924918651580802</v>
-      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
@@ -3559,69 +2798,43 @@
       <c r="B50" s="8">
         <v>1</v>
       </c>
-      <c r="C50" s="1">
-        <v>-0.59897530078887895</v>
-      </c>
-      <c r="D50" s="1">
-        <v>2.3569996356964098</v>
-      </c>
-      <c r="E50" s="1">
-        <v>-0.70700454711913996</v>
-      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="9"/>
-      <c r="C51" s="1">
-        <v>-1.3289710283279399</v>
-      </c>
-      <c r="D51" s="1">
-        <v>2.7057578563690101</v>
-      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="8">
         <v>2</v>
       </c>
-      <c r="C52" s="1">
-        <v>-0.67250257730483998</v>
-      </c>
-      <c r="D52" s="1">
-        <v>3.5115864276885902</v>
-      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="9"/>
-      <c r="C53" s="1">
-        <v>-3.0443739891052202</v>
-      </c>
-      <c r="D53" s="1">
-        <v>-0.34232163429260198</v>
-      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="8">
         <v>3</v>
       </c>
-      <c r="C54" s="1">
-        <v>1.5171325206756501</v>
-      </c>
-      <c r="D54" s="1">
-        <v>0.43526506423950101</v>
-      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="9"/>
-      <c r="C55" s="1">
-        <v>-2.2962193489074698</v>
-      </c>
-      <c r="D55" s="1">
-        <v>-0.17438523471355399</v>
-      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
@@ -3630,69 +2843,43 @@
       <c r="B56" s="8">
         <v>1</v>
       </c>
-      <c r="C56" s="1">
-        <v>-1.70358073711395</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2.4219911098480198</v>
-      </c>
-      <c r="E56" s="1">
-        <v>-3.5636575222015301</v>
-      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="9"/>
-      <c r="C57" s="1">
-        <v>-9.9958568811416598E-2</v>
-      </c>
-      <c r="D57" s="1">
-        <v>-2.54979276657104</v>
-      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="8">
         <v>2</v>
       </c>
-      <c r="C58" s="1">
-        <v>3.8382477760314901</v>
-      </c>
-      <c r="D58" s="1">
-        <v>-2.5205166339874201</v>
-      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="9"/>
-      <c r="C59" s="1">
-        <v>-0.67971986532211304</v>
-      </c>
-      <c r="D59" s="1">
-        <v>-3.2891609668731601</v>
-      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="8">
         <v>3</v>
       </c>
-      <c r="C60" s="1">
-        <v>-1.7507747411727901</v>
-      </c>
-      <c r="D60" s="1">
-        <v>2.2773973941802899</v>
-      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="9"/>
-      <c r="C61" s="1">
-        <v>4.4582104682922301</v>
-      </c>
-      <c r="D61" s="1">
-        <v>-1.760959982872</v>
-      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -3739,5 +2926,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>